<commit_message>
Schemas du lundi 24 octobre
</commit_message>
<xml_diff>
--- a/Calendrier_previsionnel.xlsx
+++ b/Calendrier_previsionnel.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="43">
   <si>
     <t>Octobre</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Backend</t>
   </si>
   <si>
-    <t>Mis en place Infrastructure</t>
-  </si>
-  <si>
     <t>Base de données</t>
   </si>
   <si>
@@ -169,6 +166,15 @@
   </si>
   <si>
     <t>E= Everybody dance now</t>
+  </si>
+  <si>
+    <t>Mise en place Infrastructure</t>
+  </si>
+  <si>
+    <t>Tache</t>
+  </si>
+  <si>
+    <t>Sous-tache</t>
   </si>
 </sst>
 </file>
@@ -919,7 +925,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -994,58 +1000,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1053,64 +1010,115 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading" xfId="1"/>
@@ -1435,10 +1443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S26"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="E18" sqref="E18:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="22.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1447,37 +1455,37 @@
     <col min="2" max="1024" width="8.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:21" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="34" t="s">
+      <c r="C1" s="69"/>
+      <c r="D1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34" t="s">
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34" t="s">
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="N1" s="34"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="34"/>
-      <c r="Q1" s="34" t="s">
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
+      <c r="P1" s="70"/>
+      <c r="Q1" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="34"/>
-    </row>
-    <row r="2" spans="1:19" ht="26.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="R1" s="70"/>
+    </row>
+    <row r="2" spans="1:21" ht="26.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1533,32 +1541,32 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="22.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="22.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="32"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="65"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="65"/>
       <c r="S3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
@@ -1582,10 +1590,10 @@
       <c r="Q4" s="9"/>
       <c r="R4" s="10"/>
       <c r="S4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="11" t="s">
         <v>12</v>
       </c>
@@ -1609,10 +1617,10 @@
       <c r="Q5" s="14"/>
       <c r="R5" s="15"/>
       <c r="S5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
@@ -1636,10 +1644,10 @@
       <c r="Q6" s="14"/>
       <c r="R6" s="15"/>
       <c r="S6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="11" t="s">
         <v>14</v>
       </c>
@@ -1663,16 +1671,16 @@
       <c r="Q7" s="14"/>
       <c r="R7" s="15"/>
     </row>
-    <row r="8" spans="1:19" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:21" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="37"/>
+      <c r="B8" s="71" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="73"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
@@ -1686,17 +1694,21 @@
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
       <c r="R8" s="15"/>
-    </row>
-    <row r="9" spans="1:19" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="T8" s="79"/>
+      <c r="U8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="37"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="73"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -1710,17 +1722,21 @@
       <c r="P9" s="14"/>
       <c r="Q9" s="14"/>
       <c r="R9" s="15"/>
-    </row>
-    <row r="10" spans="1:19" ht="22.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="T9" s="80"/>
+      <c r="U9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="22.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="18"/>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="39"/>
+      <c r="E10" s="74"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
       <c r="H10" s="19"/>
@@ -1735,42 +1751,42 @@
       <c r="Q10" s="19"/>
       <c r="R10" s="20"/>
     </row>
-    <row r="11" spans="1:19" ht="22.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" ht="22.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-      <c r="O11" s="32"/>
-      <c r="P11" s="32"/>
-      <c r="Q11" s="32"/>
-      <c r="R11" s="32"/>
-    </row>
-    <row r="12" spans="1:19" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="65"/>
+      <c r="C11" s="65"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="65"/>
+      <c r="K11" s="65"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="65"/>
+      <c r="N11" s="65"/>
+      <c r="O11" s="65"/>
+      <c r="P11" s="65"/>
+      <c r="Q11" s="65"/>
+      <c r="R11" s="65"/>
+    </row>
+    <row r="12" spans="1:21" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="21" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="B12" s="22"/>
       <c r="C12" s="9"/>
-      <c r="D12" s="78" t="s">
+      <c r="D12" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="41"/>
-      <c r="G12" s="42"/>
+      <c r="E12" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="47"/>
+      <c r="G12" s="55"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
@@ -1783,19 +1799,19 @@
       <c r="Q12" s="9"/>
       <c r="R12" s="10"/>
     </row>
-    <row r="13" spans="1:19" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:21" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="24"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
-      <c r="F13" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="44"/>
-      <c r="H13" s="45"/>
+      <c r="F13" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="53"/>
+      <c r="H13" s="75"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
       <c r="K13" s="14"/>
@@ -1807,157 +1823,157 @@
       <c r="Q13" s="14"/>
       <c r="R13" s="15"/>
     </row>
-    <row r="14" spans="1:19" ht="22.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" ht="22.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="36"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="76" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="77"/>
+      <c r="H14" s="77"/>
+      <c r="I14" s="78"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="39"/>
+    </row>
+    <row r="15" spans="1:21" ht="22.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="53"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="56"/>
-      <c r="H14" s="56"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="58"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="54"/>
-      <c r="M14" s="54"/>
-      <c r="N14" s="54"/>
-      <c r="O14" s="54"/>
-      <c r="P14" s="54"/>
-      <c r="Q14" s="54"/>
-      <c r="R14" s="59"/>
-    </row>
-    <row r="15" spans="1:19" ht="22.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="52" t="s">
+      <c r="B15" s="66"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="67"/>
+      <c r="M15" s="67"/>
+      <c r="N15" s="67"/>
+      <c r="O15" s="67"/>
+      <c r="P15" s="67"/>
+      <c r="Q15" s="67"/>
+      <c r="R15" s="68"/>
+    </row>
+    <row r="16" spans="1:21" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="63"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="64"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="64"/>
-      <c r="M15" s="64"/>
-      <c r="N15" s="64"/>
-      <c r="O15" s="64"/>
-      <c r="P15" s="64"/>
-      <c r="Q15" s="64"/>
-      <c r="R15" s="65"/>
-    </row>
-    <row r="16" spans="1:19" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="60"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="61"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="41"/>
       <c r="E16" s="62" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F16" s="62"/>
       <c r="G16" s="62"/>
       <c r="H16" s="62"/>
       <c r="I16" s="62"/>
-      <c r="J16" s="66" t="s">
-        <v>34</v>
-      </c>
-      <c r="K16" s="67"/>
-      <c r="L16" s="67"/>
-      <c r="M16" s="67"/>
-      <c r="N16" s="67"/>
-      <c r="O16" s="67"/>
-      <c r="P16" s="67"/>
-      <c r="Q16" s="67"/>
-      <c r="R16" s="68"/>
+      <c r="J16" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="K16" s="57"/>
+      <c r="L16" s="57"/>
+      <c r="M16" s="57"/>
+      <c r="N16" s="57"/>
+      <c r="O16" s="57"/>
+      <c r="P16" s="57"/>
+      <c r="Q16" s="57"/>
+      <c r="R16" s="58"/>
     </row>
     <row r="17" spans="1:18" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="24"/>
       <c r="C17" s="14"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="50" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="50"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="69" t="s">
+      <c r="D17" s="32"/>
+      <c r="E17" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="K17" s="44"/>
-      <c r="L17" s="44"/>
-      <c r="M17" s="44"/>
-      <c r="N17" s="44"/>
-      <c r="O17" s="44"/>
-      <c r="P17" s="44"/>
-      <c r="Q17" s="44"/>
-      <c r="R17" s="70"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="59" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17" s="53"/>
+      <c r="L17" s="53"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="53"/>
+      <c r="O17" s="53"/>
+      <c r="P17" s="53"/>
+      <c r="Q17" s="53"/>
+      <c r="R17" s="54"/>
     </row>
     <row r="18" spans="1:18" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="24"/>
       <c r="C18" s="14"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="51" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="72" t="s">
-        <v>36</v>
-      </c>
-      <c r="K18" s="73"/>
-      <c r="L18" s="73"/>
-      <c r="M18" s="73"/>
-      <c r="N18" s="73"/>
-      <c r="O18" s="73"/>
-      <c r="P18" s="71"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="64" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="64"/>
+      <c r="G18" s="64"/>
+      <c r="H18" s="64"/>
+      <c r="I18" s="64"/>
+      <c r="J18" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="K18" s="44"/>
+      <c r="L18" s="44"/>
+      <c r="M18" s="44"/>
+      <c r="N18" s="44"/>
+      <c r="O18" s="44"/>
+      <c r="P18" s="61"/>
       <c r="Q18" s="13"/>
       <c r="R18" s="27"/>
     </row>
     <row r="19" spans="1:18" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="24"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="49"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="34"/>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
       <c r="N19" s="13"/>
-      <c r="O19" s="74" t="s">
-        <v>36</v>
-      </c>
-      <c r="P19" s="73"/>
-      <c r="Q19" s="73"/>
-      <c r="R19" s="75"/>
+      <c r="O19" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="P19" s="44"/>
+      <c r="Q19" s="44"/>
+      <c r="R19" s="45"/>
     </row>
     <row r="20" spans="1:18" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="24"/>
       <c r="C20" s="14"/>
@@ -1972,16 +1988,16 @@
       <c r="L20" s="13"/>
       <c r="M20" s="13"/>
       <c r="N20" s="13"/>
-      <c r="O20" s="74" t="s">
-        <v>36</v>
-      </c>
-      <c r="P20" s="73"/>
-      <c r="Q20" s="73"/>
-      <c r="R20" s="75"/>
+      <c r="O20" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="P20" s="44"/>
+      <c r="Q20" s="44"/>
+      <c r="R20" s="45"/>
     </row>
     <row r="21" spans="1:18" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="24"/>
       <c r="C21" s="14"/>
@@ -1996,16 +2012,16 @@
       <c r="L21" s="13"/>
       <c r="M21" s="13"/>
       <c r="N21" s="13"/>
-      <c r="O21" s="74" t="s">
-        <v>36</v>
-      </c>
-      <c r="P21" s="73"/>
-      <c r="Q21" s="73"/>
-      <c r="R21" s="75"/>
+      <c r="O21" s="43" t="s">
+        <v>35</v>
+      </c>
+      <c r="P21" s="44"/>
+      <c r="Q21" s="44"/>
+      <c r="R21" s="45"/>
     </row>
     <row r="22" spans="1:18" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="24"/>
       <c r="C22" s="14"/>
@@ -2018,18 +2034,18 @@
       <c r="J22" s="14"/>
       <c r="K22" s="14"/>
       <c r="L22" s="14"/>
-      <c r="M22" s="43" t="s">
+      <c r="M22" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="N22" s="44"/>
-      <c r="O22" s="44"/>
-      <c r="P22" s="44"/>
-      <c r="Q22" s="44"/>
-      <c r="R22" s="70"/>
+      <c r="N22" s="53"/>
+      <c r="O22" s="53"/>
+      <c r="P22" s="53"/>
+      <c r="Q22" s="53"/>
+      <c r="R22" s="54"/>
     </row>
     <row r="23" spans="1:18" ht="22.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A23" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="17"/>
       <c r="C23" s="19"/>
@@ -2044,38 +2060,38 @@
       <c r="L23" s="19"/>
       <c r="M23" s="19"/>
       <c r="N23" s="19"/>
-      <c r="O23" s="38" t="s">
+      <c r="O23" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="P23" s="46"/>
-      <c r="Q23" s="46"/>
-      <c r="R23" s="77"/>
+      <c r="P23" s="50"/>
+      <c r="Q23" s="50"/>
+      <c r="R23" s="51"/>
     </row>
     <row r="24" spans="1:18" ht="22.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="32"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="32"/>
-      <c r="Q24" s="32"/>
-      <c r="R24" s="32"/>
+        <v>30</v>
+      </c>
+      <c r="B24" s="65"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
+      <c r="K24" s="65"/>
+      <c r="L24" s="65"/>
+      <c r="M24" s="65"/>
+      <c r="N24" s="65"/>
+      <c r="O24" s="65"/>
+      <c r="P24" s="65"/>
+      <c r="Q24" s="65"/>
+      <c r="R24" s="65"/>
     </row>
     <row r="25" spans="1:18" ht="22.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="28" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="29"/>
       <c r="C25" s="9"/>
@@ -2086,20 +2102,20 @@
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
-      <c r="K25" s="40" t="s">
-        <v>33</v>
-      </c>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="41"/>
-      <c r="P25" s="41"/>
-      <c r="Q25" s="41"/>
-      <c r="R25" s="76"/>
+      <c r="K25" s="46" t="s">
+        <v>32</v>
+      </c>
+      <c r="L25" s="47"/>
+      <c r="M25" s="47"/>
+      <c r="N25" s="47"/>
+      <c r="O25" s="47"/>
+      <c r="P25" s="47"/>
+      <c r="Q25" s="47"/>
+      <c r="R25" s="48"/>
     </row>
     <row r="26" spans="1:18" ht="22.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A26" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" s="31"/>
       <c r="C26" s="19"/>
@@ -2112,31 +2128,17 @@
       <c r="J26" s="19"/>
       <c r="K26" s="19"/>
       <c r="L26" s="19"/>
-      <c r="M26" s="38" t="s">
+      <c r="M26" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="N26" s="46"/>
-      <c r="O26" s="46"/>
-      <c r="P26" s="46"/>
-      <c r="Q26" s="46"/>
-      <c r="R26" s="77"/>
+      <c r="N26" s="50"/>
+      <c r="O26" s="50"/>
+      <c r="P26" s="50"/>
+      <c r="Q26" s="50"/>
+      <c r="R26" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="O20:R20"/>
-    <mergeCell ref="O21:R21"/>
-    <mergeCell ref="K25:R25"/>
-    <mergeCell ref="M26:R26"/>
-    <mergeCell ref="O23:R23"/>
-    <mergeCell ref="M22:R22"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="J16:R16"/>
-    <mergeCell ref="J17:R17"/>
-    <mergeCell ref="J18:P18"/>
-    <mergeCell ref="O19:R19"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="E18:I18"/>
     <mergeCell ref="B11:R11"/>
     <mergeCell ref="B15:R15"/>
     <mergeCell ref="B24:R24"/>
@@ -2151,6 +2153,20 @@
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="F13:H13"/>
     <mergeCell ref="F14:I14"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="J16:R16"/>
+    <mergeCell ref="J17:R17"/>
+    <mergeCell ref="J18:P18"/>
+    <mergeCell ref="O19:R19"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="O20:R20"/>
+    <mergeCell ref="O21:R21"/>
+    <mergeCell ref="K25:R25"/>
+    <mergeCell ref="M26:R26"/>
+    <mergeCell ref="O23:R23"/>
+    <mergeCell ref="M22:R22"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39370078740157477" bottom="0.39370078740157477" header="0" footer="0"/>
   <headerFooter>

</xml_diff>